<commit_message>
Fix the currency problem by downgrading poi.
</commit_message>
<xml_diff>
--- a/src/docs/Sample.xlsx
+++ b/src/docs/Sample.xlsx
@@ -46,9 +46,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -120,7 +119,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -138,15 +137,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Komma" xfId="6" builtinId="3"/>
     <cellStyle name="Prozent" xfId="5" builtinId="5"/>
     <cellStyle name="Prozent 2" xfId="4"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
     <cellStyle name="Standard 3" xfId="2"/>
+    <cellStyle name="Währung" xfId="6" builtinId="4"/>
     <cellStyle name="Währung 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -729,7 +728,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix #63 reset background color for cells in exportExcel
</commit_message>
<xml_diff>
--- a/src/docs/Sample.xlsx
+++ b/src/docs/Sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19320" windowHeight="10110" tabRatio="681"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19320" windowHeight="10110" tabRatio="681" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Werte" sheetId="1" r:id="rId1"/>
     <sheet name="Numerisch" sheetId="2" r:id="rId2"/>
+    <sheet name="ColAndRowSpan" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>A</t>
   </si>
@@ -92,6 +93,36 @@
   </si>
   <si>
     <t>test *bold*</t>
+  </si>
+  <si>
+    <t>ColSpan</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
@@ -197,7 +228,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -241,6 +272,10 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -781,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -967,4 +1002,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18">
+        <v>6</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>